<commit_message>
Snelle commit voor batterij op is!
</commit_message>
<xml_diff>
--- a/scape_results_19.xlsx
+++ b/scape_results_19.xlsx
@@ -494,6 +494,18 @@
           <t>1</t>
         </is>
       </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>NATIONAL WATCH</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr"/>
+      <c r="E2" t="inlineStr"/>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>NATIONAL WATCH</t>
+        </is>
+      </c>
       <c r="G2" t="inlineStr">
         <is>
           <t>CHF</t>
@@ -519,11 +531,19 @@
           <t xml:space="preserve"> May 14, 2017 </t>
         </is>
       </c>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
       <c r="N2" t="inlineStr">
         <is>
           <t xml:space="preserve"> Very good</t>
         </is>
       </c>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
+      <c r="Q2" t="inlineStr"/>
+      <c r="R2" t="inlineStr"/>
+      <c r="S2" t="inlineStr"/>
+      <c r="T2" t="inlineStr"/>
       <c r="U2" t="inlineStr">
         <is>
           <t>https://catalog.antiquorum.swiss/en/lots/national-watch-co-lot-307-1?page=0</t>
@@ -566,6 +586,18 @@
           <t>2</t>
         </is>
       </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>GALLET</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr"/>
+      <c r="E3" t="inlineStr"/>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>GALLET</t>
+        </is>
+      </c>
       <c r="G3" t="inlineStr">
         <is>
           <t>CHF</t>
@@ -591,11 +623,19 @@
           <t xml:space="preserve"> May 14, 2017 </t>
         </is>
       </c>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
       <c r="N3" t="inlineStr">
         <is>
           <t xml:space="preserve"> Very good</t>
         </is>
       </c>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
+      <c r="Q3" t="inlineStr"/>
+      <c r="R3" t="inlineStr"/>
+      <c r="S3" t="inlineStr"/>
+      <c r="T3" t="inlineStr"/>
       <c r="U3" t="inlineStr">
         <is>
           <t>https://catalog.antiquorum.swiss/en/lots/gallet-cie-lot-307-2?page=0</t>
@@ -635,6 +675,18 @@
           <t>3</t>
         </is>
       </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>HELVETIA</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr"/>
+      <c r="E4" t="inlineStr"/>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>HELVETIA</t>
+        </is>
+      </c>
       <c r="G4" t="inlineStr">
         <is>
           <t>CHF</t>
@@ -660,11 +712,19 @@
           <t xml:space="preserve"> May 14, 2017 </t>
         </is>
       </c>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
       <c r="N4" t="inlineStr">
         <is>
           <t xml:space="preserve"> Very good</t>
         </is>
       </c>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
+      <c r="Q4" t="inlineStr"/>
+      <c r="R4" t="inlineStr"/>
+      <c r="S4" t="inlineStr"/>
+      <c r="T4" t="inlineStr"/>
       <c r="U4" t="inlineStr">
         <is>
           <t>https://catalog.antiquorum.swiss/en/lots/helvetia-lot-307-3?page=0</t>

</xml_diff>